<commit_message>
more updates to plate key
</commit_message>
<xml_diff>
--- a/data-general/chlamee-acclimation-plate-key.xlsx
+++ b/data-general/chlamee-acclimation-plate-key.xlsx
@@ -27,12 +27,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>plate</t>
   </si>
   <si>
     <t>temperature</t>
+  </si>
+  <si>
+    <t>plate_key</t>
+  </si>
+  <si>
+    <t>plate3</t>
   </si>
 </sst>
 </file>
@@ -347,359 +353,620 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>22</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>29</v>
+      </c>
+      <c r="B6">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>36</v>
+      </c>
+      <c r="B7">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B8">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>28</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="B11">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>40</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
         <v>13</v>
       </c>
-      <c r="B14">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B15">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>22</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>3</v>
+      </c>
+      <c r="D16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>28</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
         <v>16</v>
       </c>
-      <c r="B17">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>31</v>
+      </c>
+      <c r="B18">
+        <v>34</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
         <v>17</v>
       </c>
-      <c r="B18">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
         <v>18</v>
       </c>
-      <c r="B19">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
         <v>19</v>
       </c>
-      <c r="B20">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21">
+        <v>16</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
         <v>20</v>
       </c>
-      <c r="B21">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>34</v>
+      </c>
+      <c r="C24">
+        <v>4</v>
+      </c>
+      <c r="D24">
         <v>23</v>
       </c>
-      <c r="B24">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
+        <v>39</v>
+      </c>
+      <c r="B25">
+        <v>40</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
         <v>24</v>
       </c>
-      <c r="B25">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
         <v>25</v>
       </c>
-      <c r="B26">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
+        <v>12</v>
+      </c>
+      <c r="B27">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
         <v>26</v>
       </c>
-      <c r="B27">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
+        <v>19</v>
+      </c>
+      <c r="B28">
+        <v>22</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
         <v>27</v>
       </c>
-      <c r="B28">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>5</v>
+      </c>
+      <c r="D29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B30">
         <v>34</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
+        <v>40</v>
+      </c>
+      <c r="B31">
+        <v>40</v>
+      </c>
+      <c r="C31">
+        <v>5</v>
+      </c>
+      <c r="D31">
         <v>30</v>
       </c>
-      <c r="B31">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="B32">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>13</v>
+      </c>
+      <c r="B33">
+        <v>16</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>22</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <v>28</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>35</v>
       </c>
       <c r="B36">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>6</v>
+      </c>
+      <c r="D36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="B37">
         <v>40</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
         <v>37</v>
       </c>
-      <c r="B38">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>14</v>
+      </c>
+      <c r="B39">
+        <v>16</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>21</v>
+      </c>
+      <c r="B40">
+        <v>22</v>
+      </c>
+      <c r="C40">
+        <v>7</v>
+      </c>
+      <c r="D40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>28</v>
+      </c>
+      <c r="B41">
+        <v>28</v>
+      </c>
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41">
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
+        <v>35</v>
+      </c>
+      <c r="B42">
+        <v>34</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
+      </c>
+      <c r="D42">
         <v>41</v>
       </c>
-      <c r="B42">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43">
         <v>40</v>
       </c>
+      <c r="C43">
+        <v>7</v>
+      </c>
+      <c r="D43">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C43">
+    <sortCondition ref="C2:C43"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>